<commit_message>
📊 Update SwaadSutra_Daily_2026-01-13.xlsx - 2026-01-13T10:11:07.641Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Daily_2026-01-13.xlsx
+++ b/reports/SwaadSutra_Daily_2026-01-13.xlsx
@@ -471,7 +471,7 @@
         <v>30</v>
       </c>
       <c r="H2" t="str">
-        <v>NEW</v>
+        <v>COOKING</v>
       </c>
       <c r="I2" t="str">
         <v>PENDING</v>
@@ -537,10 +537,10 @@
         <v>1</v>
       </c>
       <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
         <v>1</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
       </c>
       <c r="D2">
         <v>0</v>

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Daily_2026-01-13.xlsx - 2026-01-13T10:20:49.468Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Daily_2026-01-13.xlsx
+++ b/reports/SwaadSutra_Daily_2026-01-13.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -450,51 +450,95 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" t="str">
-        <v>2026-01-13 10:09</v>
+        <v>2026-01-13 10:20</v>
       </c>
       <c r="C2" t="str">
-        <v>Anuradha N</v>
+        <v>Pooja</v>
       </c>
       <c r="D2" t="str">
-        <v>B 304</v>
+        <v>A 1608</v>
       </c>
       <c r="E2" t="str">
         <v/>
       </c>
       <c r="F2" t="str">
-        <v>Til Poli x1</v>
+        <v>Wheat Chapati x1</v>
       </c>
       <c r="G2">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H2" t="str">
-        <v>COOKING</v>
+        <v>NEW</v>
       </c>
       <c r="I2" t="str">
         <v>PENDING</v>
       </c>
       <c r="J2" t="str">
+        <v>2026-01-13</v>
+      </c>
+      <c r="K2" t="str">
+        <v>15:50</v>
+      </c>
+      <c r="L2" t="str">
+        <v/>
+      </c>
+      <c r="M2" t="str">
+        <v/>
+      </c>
+      <c r="N2" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="str">
+        <v>2026-01-13 10:09</v>
+      </c>
+      <c r="C3" t="str">
+        <v>Anuradha N</v>
+      </c>
+      <c r="D3" t="str">
+        <v>B 304</v>
+      </c>
+      <c r="E3" t="str">
+        <v/>
+      </c>
+      <c r="F3" t="str">
+        <v>Til Poli x1</v>
+      </c>
+      <c r="G3">
+        <v>30</v>
+      </c>
+      <c r="H3" t="str">
+        <v>COOKING</v>
+      </c>
+      <c r="I3" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J3" t="str">
         <v>2026-01-14</v>
       </c>
-      <c r="K2" t="str">
+      <c r="K3" t="str">
         <v>16:45</v>
       </c>
-      <c r="L2" t="str">
-        <v/>
-      </c>
-      <c r="M2" t="str">
-        <v/>
-      </c>
-      <c r="N2" t="str">
+      <c r="L3" t="str">
+        <v/>
+      </c>
+      <c r="M3" t="str">
+        <v/>
+      </c>
+      <c r="N3" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N3"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -534,10 +578,10 @@
     </row>
     <row r="2">
       <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
         <v>1</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -552,7 +596,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -567,7 +611,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -585,18 +629,29 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Til Poli</v>
+        <v>Wheat Chapati</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Til Poli</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
         <v>30</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
📊 Update SwaadSutra_Daily_2026-01-13.xlsx - 2026-01-13T11:15:13.638Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Daily_2026-01-13.xlsx
+++ b/reports/SwaadSutra_Daily_2026-01-13.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -450,25 +450,25 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" t="str">
-        <v>2026-01-13 10:20</v>
+        <v>2026-01-13 11:15</v>
       </c>
       <c r="C2" t="str">
-        <v>Pooja</v>
+        <v>Ajay Dwarkunde</v>
       </c>
       <c r="D2" t="str">
-        <v>A 1608</v>
+        <v>b-703</v>
       </c>
       <c r="E2" t="str">
-        <v/>
+        <v>8087172173</v>
       </c>
       <c r="F2" t="str">
-        <v>Wheat Chapati x1</v>
+        <v>Pohe x1</v>
       </c>
       <c r="G2">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="H2" t="str">
         <v>NEW</v>
@@ -480,7 +480,7 @@
         <v>2026-01-13</v>
       </c>
       <c r="K2" t="str">
-        <v>15:50</v>
+        <v>18:50</v>
       </c>
       <c r="L2" t="str">
         <v/>
@@ -494,51 +494,95 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="str">
-        <v>2026-01-13 10:09</v>
+        <v>2026-01-13 10:20</v>
       </c>
       <c r="C3" t="str">
-        <v>Anuradha N</v>
+        <v>Pooja</v>
       </c>
       <c r="D3" t="str">
-        <v>B 304</v>
+        <v>A 1608</v>
       </c>
       <c r="E3" t="str">
         <v/>
       </c>
       <c r="F3" t="str">
-        <v>Til Poli x1</v>
+        <v>Wheat Chapati x1</v>
       </c>
       <c r="G3">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H3" t="str">
-        <v>COOKING</v>
+        <v>NEW</v>
       </c>
       <c r="I3" t="str">
         <v>PENDING</v>
       </c>
       <c r="J3" t="str">
+        <v>2026-01-13</v>
+      </c>
+      <c r="K3" t="str">
+        <v>15:50</v>
+      </c>
+      <c r="L3" t="str">
+        <v/>
+      </c>
+      <c r="M3" t="str">
+        <v/>
+      </c>
+      <c r="N3" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="str">
+        <v>2026-01-13 10:09</v>
+      </c>
+      <c r="C4" t="str">
+        <v>Anuradha N</v>
+      </c>
+      <c r="D4" t="str">
+        <v>B 304</v>
+      </c>
+      <c r="E4" t="str">
+        <v/>
+      </c>
+      <c r="F4" t="str">
+        <v>Til Poli x1</v>
+      </c>
+      <c r="G4">
+        <v>30</v>
+      </c>
+      <c r="H4" t="str">
+        <v>COOKING</v>
+      </c>
+      <c r="I4" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J4" t="str">
         <v>2026-01-14</v>
       </c>
-      <c r="K3" t="str">
+      <c r="K4" t="str">
         <v>16:45</v>
       </c>
-      <c r="L3" t="str">
-        <v/>
-      </c>
-      <c r="M3" t="str">
-        <v/>
-      </c>
-      <c r="N3" t="str">
+      <c r="L4" t="str">
+        <v/>
+      </c>
+      <c r="M4" t="str">
+        <v/>
+      </c>
+      <c r="N4" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N4"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -578,10 +622,10 @@
     </row>
     <row r="2">
       <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2">
         <v>2</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -596,7 +640,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>45</v>
+        <v>75</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -611,7 +655,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -629,29 +673,40 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Wheat Chapati</v>
+        <v>Pohe</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Til Poli</v>
+        <v>Wheat Chapati</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Til Poli</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
         <v>30</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
📊 Update SwaadSutra_Daily_2026-01-13.xlsx - 2026-01-13T16:39:08.475Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Daily_2026-01-13.xlsx
+++ b/reports/SwaadSutra_Daily_2026-01-13.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -450,25 +450,25 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" t="str">
-        <v>2026-01-13 11:15</v>
+        <v>2026-01-13 16:39</v>
       </c>
       <c r="C2" t="str">
-        <v>Ajay Dwarkunde</v>
+        <v>Pooja</v>
       </c>
       <c r="D2" t="str">
-        <v>b-703</v>
+        <v>A1608</v>
       </c>
       <c r="E2" t="str">
-        <v>8087172173</v>
+        <v>9096648553</v>
       </c>
       <c r="F2" t="str">
-        <v>Pohe x1</v>
+        <v>Onion Pakoda (Kanda Bhaje) x1</v>
       </c>
       <c r="G2">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="H2" t="str">
         <v>NEW</v>
@@ -477,10 +477,10 @@
         <v>PENDING</v>
       </c>
       <c r="J2" t="str">
-        <v>2026-01-13</v>
+        <v>2026-01-14</v>
       </c>
       <c r="K2" t="str">
-        <v>18:50</v>
+        <v>22:09</v>
       </c>
       <c r="L2" t="str">
         <v/>
@@ -494,25 +494,25 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" t="str">
-        <v>2026-01-13 10:20</v>
+        <v>2026-01-13 11:15</v>
       </c>
       <c r="C3" t="str">
-        <v>Pooja</v>
+        <v>Ajay Dwarkunde</v>
       </c>
       <c r="D3" t="str">
-        <v>A 1608</v>
+        <v>b-703</v>
       </c>
       <c r="E3" t="str">
-        <v/>
+        <v>8087172173</v>
       </c>
       <c r="F3" t="str">
-        <v>Wheat Chapati x1</v>
+        <v>Pohe x1</v>
       </c>
       <c r="G3">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="H3" t="str">
         <v>NEW</v>
@@ -524,7 +524,7 @@
         <v>2026-01-13</v>
       </c>
       <c r="K3" t="str">
-        <v>15:50</v>
+        <v>18:50</v>
       </c>
       <c r="L3" t="str">
         <v/>
@@ -538,51 +538,95 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" t="str">
-        <v>2026-01-13 10:09</v>
+        <v>2026-01-13 10:20</v>
       </c>
       <c r="C4" t="str">
-        <v>Anuradha N</v>
+        <v>Pooja</v>
       </c>
       <c r="D4" t="str">
-        <v>B 304</v>
+        <v>A 1608</v>
       </c>
       <c r="E4" t="str">
         <v/>
       </c>
       <c r="F4" t="str">
-        <v>Til Poli x1</v>
+        <v>Wheat Chapati x1</v>
       </c>
       <c r="G4">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H4" t="str">
-        <v>COOKING</v>
+        <v>NEW</v>
       </c>
       <c r="I4" t="str">
         <v>PENDING</v>
       </c>
       <c r="J4" t="str">
+        <v>2026-01-13</v>
+      </c>
+      <c r="K4" t="str">
+        <v>15:50</v>
+      </c>
+      <c r="L4" t="str">
+        <v/>
+      </c>
+      <c r="M4" t="str">
+        <v/>
+      </c>
+      <c r="N4" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="str">
+        <v>2026-01-13 10:09</v>
+      </c>
+      <c r="C5" t="str">
+        <v>Anuradha N</v>
+      </c>
+      <c r="D5" t="str">
+        <v>B 304</v>
+      </c>
+      <c r="E5" t="str">
+        <v/>
+      </c>
+      <c r="F5" t="str">
+        <v>Til Poli x1</v>
+      </c>
+      <c r="G5">
+        <v>30</v>
+      </c>
+      <c r="H5" t="str">
+        <v>COOKING</v>
+      </c>
+      <c r="I5" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J5" t="str">
         <v>2026-01-14</v>
       </c>
-      <c r="K4" t="str">
+      <c r="K5" t="str">
         <v>16:45</v>
       </c>
-      <c r="L4" t="str">
-        <v/>
-      </c>
-      <c r="M4" t="str">
-        <v/>
-      </c>
-      <c r="N4" t="str">
+      <c r="L5" t="str">
+        <v/>
+      </c>
+      <c r="M5" t="str">
+        <v/>
+      </c>
+      <c r="N5" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N5"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -622,10 +666,10 @@
     </row>
     <row r="2">
       <c r="A2">
+        <v>4</v>
+      </c>
+      <c r="B2">
         <v>3</v>
-      </c>
-      <c r="B2">
-        <v>2</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -640,7 +684,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>75</v>
+        <v>135</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -655,7 +699,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -673,40 +717,51 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Pohe</v>
+        <v>Onion Pakoda (Kanda Bhaje)</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2">
-        <v>30</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Wheat Chapati</v>
+        <v>Pohe</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Til Poli</v>
+        <v>Wheat Chapati</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Til Poli</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
         <v>30</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
📊 Update SwaadSutra_Daily_2026-01-13.xlsx - 2026-01-13T16:40:53.588Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Daily_2026-01-13.xlsx
+++ b/reports/SwaadSutra_Daily_2026-01-13.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -450,25 +450,25 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" t="str">
-        <v>2026-01-13 16:39</v>
+        <v>2026-01-13 16:40</v>
       </c>
       <c r="C2" t="str">
-        <v>Pooja</v>
+        <v>Sagar Borse</v>
       </c>
       <c r="D2" t="str">
-        <v>A1608</v>
+        <v>A-1608</v>
       </c>
       <c r="E2" t="str">
-        <v>9096648553</v>
+        <v>7588930329</v>
       </c>
       <c r="F2" t="str">
-        <v>Onion Pakoda (Kanda Bhaje) x1</v>
+        <v>Til Poli x1</v>
       </c>
       <c r="G2">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="H2" t="str">
         <v>NEW</v>
@@ -480,7 +480,7 @@
         <v>2026-01-14</v>
       </c>
       <c r="K2" t="str">
-        <v>22:09</v>
+        <v>10:00</v>
       </c>
       <c r="L2" t="str">
         <v/>
@@ -494,25 +494,25 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" t="str">
-        <v>2026-01-13 11:15</v>
+        <v>2026-01-13 16:39</v>
       </c>
       <c r="C3" t="str">
-        <v>Ajay Dwarkunde</v>
+        <v>Pooja</v>
       </c>
       <c r="D3" t="str">
-        <v>b-703</v>
+        <v>A1608</v>
       </c>
       <c r="E3" t="str">
-        <v>8087172173</v>
+        <v>9096648553</v>
       </c>
       <c r="F3" t="str">
-        <v>Pohe x1</v>
+        <v>Onion Pakoda (Kanda Bhaje) x1</v>
       </c>
       <c r="G3">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="H3" t="str">
         <v>NEW</v>
@@ -521,10 +521,10 @@
         <v>PENDING</v>
       </c>
       <c r="J3" t="str">
-        <v>2026-01-13</v>
+        <v>2026-01-14</v>
       </c>
       <c r="K3" t="str">
-        <v>18:50</v>
+        <v>22:09</v>
       </c>
       <c r="L3" t="str">
         <v/>
@@ -538,25 +538,25 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" t="str">
-        <v>2026-01-13 10:20</v>
+        <v>2026-01-13 11:15</v>
       </c>
       <c r="C4" t="str">
-        <v>Pooja</v>
+        <v>Ajay Dwarkunde</v>
       </c>
       <c r="D4" t="str">
-        <v>A 1608</v>
+        <v>b-703</v>
       </c>
       <c r="E4" t="str">
-        <v/>
+        <v>8087172173</v>
       </c>
       <c r="F4" t="str">
-        <v>Wheat Chapati x1</v>
+        <v>Pohe x1</v>
       </c>
       <c r="G4">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="H4" t="str">
         <v>NEW</v>
@@ -568,7 +568,7 @@
         <v>2026-01-13</v>
       </c>
       <c r="K4" t="str">
-        <v>15:50</v>
+        <v>18:50</v>
       </c>
       <c r="L4" t="str">
         <v/>
@@ -582,51 +582,95 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5" t="str">
-        <v>2026-01-13 10:09</v>
+        <v>2026-01-13 10:20</v>
       </c>
       <c r="C5" t="str">
-        <v>Anuradha N</v>
+        <v>Pooja</v>
       </c>
       <c r="D5" t="str">
-        <v>B 304</v>
+        <v>A 1608</v>
       </c>
       <c r="E5" t="str">
         <v/>
       </c>
       <c r="F5" t="str">
-        <v>Til Poli x1</v>
+        <v>Wheat Chapati x1</v>
       </c>
       <c r="G5">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H5" t="str">
-        <v>COOKING</v>
+        <v>NEW</v>
       </c>
       <c r="I5" t="str">
         <v>PENDING</v>
       </c>
       <c r="J5" t="str">
+        <v>2026-01-13</v>
+      </c>
+      <c r="K5" t="str">
+        <v>15:50</v>
+      </c>
+      <c r="L5" t="str">
+        <v/>
+      </c>
+      <c r="M5" t="str">
+        <v/>
+      </c>
+      <c r="N5" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="str">
+        <v>2026-01-13 10:09</v>
+      </c>
+      <c r="C6" t="str">
+        <v>Anuradha N</v>
+      </c>
+      <c r="D6" t="str">
+        <v>B 304</v>
+      </c>
+      <c r="E6" t="str">
+        <v/>
+      </c>
+      <c r="F6" t="str">
+        <v>Til Poli x1</v>
+      </c>
+      <c r="G6">
+        <v>30</v>
+      </c>
+      <c r="H6" t="str">
+        <v>COOKING</v>
+      </c>
+      <c r="I6" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J6" t="str">
         <v>2026-01-14</v>
       </c>
-      <c r="K5" t="str">
+      <c r="K6" t="str">
         <v>16:45</v>
       </c>
-      <c r="L5" t="str">
-        <v/>
-      </c>
-      <c r="M5" t="str">
-        <v/>
-      </c>
-      <c r="N5" t="str">
+      <c r="L6" t="str">
+        <v/>
+      </c>
+      <c r="M6" t="str">
+        <v/>
+      </c>
+      <c r="N6" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N6"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -666,10 +710,10 @@
     </row>
     <row r="2">
       <c r="A2">
+        <v>5</v>
+      </c>
+      <c r="B2">
         <v>4</v>
-      </c>
-      <c r="B2">
-        <v>3</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -684,7 +728,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>135</v>
+        <v>165</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -717,10 +761,10 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Onion Pakoda (Kanda Bhaje)</v>
+        <v>Til Poli</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2">
         <v>60</v>
@@ -728,35 +772,35 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Pohe</v>
+        <v>Onion Pakoda (Kanda Bhaje)</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3">
-        <v>30</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Wheat Chapati</v>
+        <v>Pohe</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Til Poli</v>
+        <v>Wheat Chapati</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5">
-        <v>30</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Daily_2026-01-13.xlsx - 2026-01-13T16:41:26.396Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Daily_2026-01-13.xlsx
+++ b/reports/SwaadSutra_Daily_2026-01-13.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -450,25 +450,25 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="str">
-        <v>2026-01-13 16:40</v>
+        <v>2026-01-13 16:41</v>
       </c>
       <c r="C2" t="str">
-        <v>Sagar Borse</v>
+        <v>Pooja</v>
       </c>
       <c r="D2" t="str">
-        <v>A-1608</v>
+        <v>saf</v>
       </c>
       <c r="E2" t="str">
-        <v>7588930329</v>
+        <v>9096648553</v>
       </c>
       <c r="F2" t="str">
-        <v>Til Poli x1</v>
+        <v>Wheat Chapati x1</v>
       </c>
       <c r="G2">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H2" t="str">
         <v>NEW</v>
@@ -477,10 +477,10 @@
         <v>PENDING</v>
       </c>
       <c r="J2" t="str">
-        <v>2026-01-14</v>
+        <v>2026-01-15</v>
       </c>
       <c r="K2" t="str">
-        <v>10:00</v>
+        <v>10:12</v>
       </c>
       <c r="L2" t="str">
         <v/>
@@ -494,25 +494,25 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" t="str">
-        <v>2026-01-13 16:39</v>
+        <v>2026-01-13 16:40</v>
       </c>
       <c r="C3" t="str">
-        <v>Pooja</v>
+        <v>Sagar Borse</v>
       </c>
       <c r="D3" t="str">
-        <v>A1608</v>
+        <v>A-1608</v>
       </c>
       <c r="E3" t="str">
-        <v>9096648553</v>
+        <v>7588930329</v>
       </c>
       <c r="F3" t="str">
-        <v>Onion Pakoda (Kanda Bhaje) x1</v>
+        <v>Til Poli x1</v>
       </c>
       <c r="G3">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="H3" t="str">
         <v>NEW</v>
@@ -524,7 +524,7 @@
         <v>2026-01-14</v>
       </c>
       <c r="K3" t="str">
-        <v>22:09</v>
+        <v>10:00</v>
       </c>
       <c r="L3" t="str">
         <v/>
@@ -538,25 +538,25 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" t="str">
-        <v>2026-01-13 11:15</v>
+        <v>2026-01-13 16:39</v>
       </c>
       <c r="C4" t="str">
-        <v>Ajay Dwarkunde</v>
+        <v>Pooja</v>
       </c>
       <c r="D4" t="str">
-        <v>b-703</v>
+        <v>A1608</v>
       </c>
       <c r="E4" t="str">
-        <v>8087172173</v>
+        <v>9096648553</v>
       </c>
       <c r="F4" t="str">
-        <v>Pohe x1</v>
+        <v>Onion Pakoda (Kanda Bhaje) x1</v>
       </c>
       <c r="G4">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="H4" t="str">
         <v>NEW</v>
@@ -565,10 +565,10 @@
         <v>PENDING</v>
       </c>
       <c r="J4" t="str">
-        <v>2026-01-13</v>
+        <v>2026-01-14</v>
       </c>
       <c r="K4" t="str">
-        <v>18:50</v>
+        <v>22:09</v>
       </c>
       <c r="L4" t="str">
         <v/>
@@ -582,25 +582,25 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B5" t="str">
-        <v>2026-01-13 10:20</v>
+        <v>2026-01-13 11:15</v>
       </c>
       <c r="C5" t="str">
-        <v>Pooja</v>
+        <v>Ajay Dwarkunde</v>
       </c>
       <c r="D5" t="str">
-        <v>A 1608</v>
+        <v>b-703</v>
       </c>
       <c r="E5" t="str">
-        <v/>
+        <v>8087172173</v>
       </c>
       <c r="F5" t="str">
-        <v>Wheat Chapati x1</v>
+        <v>Pohe x1</v>
       </c>
       <c r="G5">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="H5" t="str">
         <v>NEW</v>
@@ -612,7 +612,7 @@
         <v>2026-01-13</v>
       </c>
       <c r="K5" t="str">
-        <v>15:50</v>
+        <v>18:50</v>
       </c>
       <c r="L5" t="str">
         <v/>
@@ -626,51 +626,95 @@
     </row>
     <row r="6">
       <c r="A6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B6" t="str">
-        <v>2026-01-13 10:09</v>
+        <v>2026-01-13 10:20</v>
       </c>
       <c r="C6" t="str">
-        <v>Anuradha N</v>
+        <v>Pooja</v>
       </c>
       <c r="D6" t="str">
-        <v>B 304</v>
+        <v>A 1608</v>
       </c>
       <c r="E6" t="str">
         <v/>
       </c>
       <c r="F6" t="str">
-        <v>Til Poli x1</v>
+        <v>Wheat Chapati x1</v>
       </c>
       <c r="G6">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H6" t="str">
-        <v>COOKING</v>
+        <v>NEW</v>
       </c>
       <c r="I6" t="str">
         <v>PENDING</v>
       </c>
       <c r="J6" t="str">
+        <v>2026-01-13</v>
+      </c>
+      <c r="K6" t="str">
+        <v>15:50</v>
+      </c>
+      <c r="L6" t="str">
+        <v/>
+      </c>
+      <c r="M6" t="str">
+        <v/>
+      </c>
+      <c r="N6" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" t="str">
+        <v>2026-01-13 10:09</v>
+      </c>
+      <c r="C7" t="str">
+        <v>Anuradha N</v>
+      </c>
+      <c r="D7" t="str">
+        <v>B 304</v>
+      </c>
+      <c r="E7" t="str">
+        <v/>
+      </c>
+      <c r="F7" t="str">
+        <v>Til Poli x1</v>
+      </c>
+      <c r="G7">
+        <v>30</v>
+      </c>
+      <c r="H7" t="str">
+        <v>COOKING</v>
+      </c>
+      <c r="I7" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J7" t="str">
         <v>2026-01-14</v>
       </c>
-      <c r="K6" t="str">
+      <c r="K7" t="str">
         <v>16:45</v>
       </c>
-      <c r="L6" t="str">
-        <v/>
-      </c>
-      <c r="M6" t="str">
-        <v/>
-      </c>
-      <c r="N6" t="str">
+      <c r="L7" t="str">
+        <v/>
+      </c>
+      <c r="M7" t="str">
+        <v/>
+      </c>
+      <c r="N7" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N7"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -710,10 +754,10 @@
     </row>
     <row r="2">
       <c r="A2">
+        <v>6</v>
+      </c>
+      <c r="B2">
         <v>5</v>
-      </c>
-      <c r="B2">
-        <v>4</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -728,7 +772,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>165</v>
+        <v>180</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -761,21 +805,21 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Til Poli</v>
+        <v>Wheat Chapati</v>
       </c>
       <c r="B2">
         <v>2</v>
       </c>
       <c r="C2">
-        <v>60</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Onion Pakoda (Kanda Bhaje)</v>
+        <v>Til Poli</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <v>60</v>
@@ -783,24 +827,24 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Pohe</v>
+        <v>Onion Pakoda (Kanda Bhaje)</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4">
-        <v>30</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Wheat Chapati</v>
+        <v>Pohe</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Daily_2026-01-13.xlsx - 2026-01-13T16:54:50.847Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Daily_2026-01-13.xlsx
+++ b/reports/SwaadSutra_Daily_2026-01-13.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -450,16 +450,16 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" t="str">
-        <v>2026-01-13 16:41</v>
+        <v>2026-01-13 16:54</v>
       </c>
       <c r="C2" t="str">
         <v>Pooja</v>
       </c>
       <c r="D2" t="str">
-        <v>saf</v>
+        <v>a14</v>
       </c>
       <c r="E2" t="str">
         <v>9096648553</v>
@@ -477,10 +477,10 @@
         <v>PENDING</v>
       </c>
       <c r="J2" t="str">
-        <v>2026-01-15</v>
+        <v/>
       </c>
       <c r="K2" t="str">
-        <v>10:12</v>
+        <v/>
       </c>
       <c r="L2" t="str">
         <v/>
@@ -494,25 +494,25 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" t="str">
-        <v>2026-01-13 16:40</v>
+        <v>2026-01-13 16:41</v>
       </c>
       <c r="C3" t="str">
-        <v>Sagar Borse</v>
+        <v>Pooja</v>
       </c>
       <c r="D3" t="str">
-        <v>A-1608</v>
+        <v>saf</v>
       </c>
       <c r="E3" t="str">
-        <v>7588930329</v>
+        <v>9096648553</v>
       </c>
       <c r="F3" t="str">
-        <v>Til Poli x1</v>
+        <v>Wheat Chapati x1</v>
       </c>
       <c r="G3">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H3" t="str">
         <v>NEW</v>
@@ -521,10 +521,10 @@
         <v>PENDING</v>
       </c>
       <c r="J3" t="str">
-        <v>2026-01-14</v>
+        <v>2026-01-15</v>
       </c>
       <c r="K3" t="str">
-        <v>10:00</v>
+        <v>10:12</v>
       </c>
       <c r="L3" t="str">
         <v/>
@@ -538,25 +538,25 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" t="str">
-        <v>2026-01-13 16:39</v>
+        <v>2026-01-13 16:40</v>
       </c>
       <c r="C4" t="str">
-        <v>Pooja</v>
+        <v>Sagar Borse</v>
       </c>
       <c r="D4" t="str">
-        <v>A1608</v>
+        <v>A-1608</v>
       </c>
       <c r="E4" t="str">
-        <v>9096648553</v>
+        <v>7588930329</v>
       </c>
       <c r="F4" t="str">
-        <v>Onion Pakoda (Kanda Bhaje) x1</v>
+        <v>Til Poli x1</v>
       </c>
       <c r="G4">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="H4" t="str">
         <v>NEW</v>
@@ -568,7 +568,7 @@
         <v>2026-01-14</v>
       </c>
       <c r="K4" t="str">
-        <v>22:09</v>
+        <v>10:00</v>
       </c>
       <c r="L4" t="str">
         <v/>
@@ -582,25 +582,25 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" t="str">
-        <v>2026-01-13 11:15</v>
+        <v>2026-01-13 16:39</v>
       </c>
       <c r="C5" t="str">
-        <v>Ajay Dwarkunde</v>
+        <v>Pooja</v>
       </c>
       <c r="D5" t="str">
-        <v>b-703</v>
+        <v>A1608</v>
       </c>
       <c r="E5" t="str">
-        <v>8087172173</v>
+        <v>9096648553</v>
       </c>
       <c r="F5" t="str">
-        <v>Pohe x1</v>
+        <v>Onion Pakoda (Kanda Bhaje) x1</v>
       </c>
       <c r="G5">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="H5" t="str">
         <v>NEW</v>
@@ -609,10 +609,10 @@
         <v>PENDING</v>
       </c>
       <c r="J5" t="str">
-        <v>2026-01-13</v>
+        <v>2026-01-14</v>
       </c>
       <c r="K5" t="str">
-        <v>18:50</v>
+        <v>22:09</v>
       </c>
       <c r="L5" t="str">
         <v/>
@@ -626,25 +626,25 @@
     </row>
     <row r="6">
       <c r="A6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B6" t="str">
-        <v>2026-01-13 10:20</v>
+        <v>2026-01-13 11:15</v>
       </c>
       <c r="C6" t="str">
-        <v>Pooja</v>
+        <v>Ajay Dwarkunde</v>
       </c>
       <c r="D6" t="str">
-        <v>A 1608</v>
+        <v>b-703</v>
       </c>
       <c r="E6" t="str">
-        <v/>
+        <v>8087172173</v>
       </c>
       <c r="F6" t="str">
-        <v>Wheat Chapati x1</v>
+        <v>Pohe x1</v>
       </c>
       <c r="G6">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="H6" t="str">
         <v>NEW</v>
@@ -656,7 +656,7 @@
         <v>2026-01-13</v>
       </c>
       <c r="K6" t="str">
-        <v>15:50</v>
+        <v>18:50</v>
       </c>
       <c r="L6" t="str">
         <v/>
@@ -670,51 +670,95 @@
     </row>
     <row r="7">
       <c r="A7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B7" t="str">
-        <v>2026-01-13 10:09</v>
+        <v>2026-01-13 10:20</v>
       </c>
       <c r="C7" t="str">
-        <v>Anuradha N</v>
+        <v>Pooja</v>
       </c>
       <c r="D7" t="str">
-        <v>B 304</v>
+        <v>A 1608</v>
       </c>
       <c r="E7" t="str">
         <v/>
       </c>
       <c r="F7" t="str">
-        <v>Til Poli x1</v>
+        <v>Wheat Chapati x1</v>
       </c>
       <c r="G7">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H7" t="str">
-        <v>COOKING</v>
+        <v>NEW</v>
       </c>
       <c r="I7" t="str">
         <v>PENDING</v>
       </c>
       <c r="J7" t="str">
+        <v>2026-01-13</v>
+      </c>
+      <c r="K7" t="str">
+        <v>15:50</v>
+      </c>
+      <c r="L7" t="str">
+        <v/>
+      </c>
+      <c r="M7" t="str">
+        <v/>
+      </c>
+      <c r="N7" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" t="str">
+        <v>2026-01-13 10:09</v>
+      </c>
+      <c r="C8" t="str">
+        <v>Anuradha N</v>
+      </c>
+      <c r="D8" t="str">
+        <v>B 304</v>
+      </c>
+      <c r="E8" t="str">
+        <v/>
+      </c>
+      <c r="F8" t="str">
+        <v>Til Poli x1</v>
+      </c>
+      <c r="G8">
+        <v>30</v>
+      </c>
+      <c r="H8" t="str">
+        <v>COOKING</v>
+      </c>
+      <c r="I8" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J8" t="str">
         <v>2026-01-14</v>
       </c>
-      <c r="K7" t="str">
+      <c r="K8" t="str">
         <v>16:45</v>
       </c>
-      <c r="L7" t="str">
-        <v/>
-      </c>
-      <c r="M7" t="str">
-        <v/>
-      </c>
-      <c r="N7" t="str">
+      <c r="L8" t="str">
+        <v/>
+      </c>
+      <c r="M8" t="str">
+        <v/>
+      </c>
+      <c r="N8" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N8"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -754,10 +798,10 @@
     </row>
     <row r="2">
       <c r="A2">
+        <v>7</v>
+      </c>
+      <c r="B2">
         <v>6</v>
-      </c>
-      <c r="B2">
-        <v>5</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -772,7 +816,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>180</v>
+        <v>195</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -808,10 +852,10 @@
         <v>Wheat Chapati</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2">
-        <v>30</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Daily_2026-01-13.xlsx - 2026-01-13T18:59:41.700Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Daily_2026-01-13.xlsx
+++ b/reports/SwaadSutra_Daily_2026-01-13.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -450,25 +450,25 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" t="str">
-        <v>2026-01-13 16:54</v>
+        <v>2026-01-13 18:59</v>
       </c>
       <c r="C2" t="str">
-        <v>Pooja</v>
+        <v>Sagar Borse</v>
       </c>
       <c r="D2" t="str">
-        <v>a14</v>
+        <v>A-1608</v>
       </c>
       <c r="E2" t="str">
-        <v>9096648553</v>
+        <v>7588930329</v>
       </c>
       <c r="F2" t="str">
-        <v>Wheat Chapati x1</v>
+        <v>Jawar Bhakari x1</v>
       </c>
       <c r="G2">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H2" t="str">
         <v>NEW</v>
@@ -477,10 +477,10 @@
         <v>PENDING</v>
       </c>
       <c r="J2" t="str">
-        <v/>
+        <v>2026-01-16</v>
       </c>
       <c r="K2" t="str">
-        <v/>
+        <v>10:00</v>
       </c>
       <c r="L2" t="str">
         <v/>
@@ -494,16 +494,16 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" t="str">
-        <v>2026-01-13 16:41</v>
+        <v>2026-01-13 16:54</v>
       </c>
       <c r="C3" t="str">
         <v>Pooja</v>
       </c>
       <c r="D3" t="str">
-        <v>saf</v>
+        <v>a14</v>
       </c>
       <c r="E3" t="str">
         <v>9096648553</v>
@@ -521,10 +521,10 @@
         <v>PENDING</v>
       </c>
       <c r="J3" t="str">
-        <v>2026-01-15</v>
+        <v/>
       </c>
       <c r="K3" t="str">
-        <v>10:12</v>
+        <v/>
       </c>
       <c r="L3" t="str">
         <v/>
@@ -538,25 +538,25 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" t="str">
-        <v>2026-01-13 16:40</v>
+        <v>2026-01-13 16:41</v>
       </c>
       <c r="C4" t="str">
-        <v>Sagar Borse</v>
+        <v>Pooja</v>
       </c>
       <c r="D4" t="str">
-        <v>A-1608</v>
+        <v>saf</v>
       </c>
       <c r="E4" t="str">
-        <v>7588930329</v>
+        <v>9096648553</v>
       </c>
       <c r="F4" t="str">
-        <v>Til Poli x1</v>
+        <v>Wheat Chapati x1</v>
       </c>
       <c r="G4">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H4" t="str">
         <v>NEW</v>
@@ -565,10 +565,10 @@
         <v>PENDING</v>
       </c>
       <c r="J4" t="str">
-        <v>2026-01-14</v>
+        <v>2026-01-15</v>
       </c>
       <c r="K4" t="str">
-        <v>10:00</v>
+        <v>10:12</v>
       </c>
       <c r="L4" t="str">
         <v/>
@@ -582,25 +582,25 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" t="str">
-        <v>2026-01-13 16:39</v>
+        <v>2026-01-13 16:40</v>
       </c>
       <c r="C5" t="str">
-        <v>Pooja</v>
+        <v>Sagar Borse</v>
       </c>
       <c r="D5" t="str">
-        <v>A1608</v>
+        <v>A-1608</v>
       </c>
       <c r="E5" t="str">
-        <v>9096648553</v>
+        <v>7588930329</v>
       </c>
       <c r="F5" t="str">
-        <v>Onion Pakoda (Kanda Bhaje) x1</v>
+        <v>Til Poli x1</v>
       </c>
       <c r="G5">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="H5" t="str">
         <v>NEW</v>
@@ -612,7 +612,7 @@
         <v>2026-01-14</v>
       </c>
       <c r="K5" t="str">
-        <v>22:09</v>
+        <v>10:00</v>
       </c>
       <c r="L5" t="str">
         <v/>
@@ -626,25 +626,25 @@
     </row>
     <row r="6">
       <c r="A6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B6" t="str">
-        <v>2026-01-13 11:15</v>
+        <v>2026-01-13 16:39</v>
       </c>
       <c r="C6" t="str">
-        <v>Ajay Dwarkunde</v>
+        <v>Pooja</v>
       </c>
       <c r="D6" t="str">
-        <v>b-703</v>
+        <v>A1608</v>
       </c>
       <c r="E6" t="str">
-        <v>8087172173</v>
+        <v>9096648553</v>
       </c>
       <c r="F6" t="str">
-        <v>Pohe x1</v>
+        <v>Onion Pakoda (Kanda Bhaje) x1</v>
       </c>
       <c r="G6">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="H6" t="str">
         <v>NEW</v>
@@ -653,10 +653,10 @@
         <v>PENDING</v>
       </c>
       <c r="J6" t="str">
-        <v>2026-01-13</v>
+        <v>2026-01-14</v>
       </c>
       <c r="K6" t="str">
-        <v>18:50</v>
+        <v>22:09</v>
       </c>
       <c r="L6" t="str">
         <v/>
@@ -670,25 +670,25 @@
     </row>
     <row r="7">
       <c r="A7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B7" t="str">
-        <v>2026-01-13 10:20</v>
+        <v>2026-01-13 11:15</v>
       </c>
       <c r="C7" t="str">
-        <v>Pooja</v>
+        <v>Ajay Dwarkunde</v>
       </c>
       <c r="D7" t="str">
-        <v>A 1608</v>
+        <v>b-703</v>
       </c>
       <c r="E7" t="str">
-        <v/>
+        <v>8087172173</v>
       </c>
       <c r="F7" t="str">
-        <v>Wheat Chapati x1</v>
+        <v>Pohe x1</v>
       </c>
       <c r="G7">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="H7" t="str">
         <v>NEW</v>
@@ -700,7 +700,7 @@
         <v>2026-01-13</v>
       </c>
       <c r="K7" t="str">
-        <v>15:50</v>
+        <v>18:50</v>
       </c>
       <c r="L7" t="str">
         <v/>
@@ -714,51 +714,95 @@
     </row>
     <row r="8">
       <c r="A8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B8" t="str">
-        <v>2026-01-13 10:09</v>
+        <v>2026-01-13 10:20</v>
       </c>
       <c r="C8" t="str">
-        <v>Anuradha N</v>
+        <v>Pooja</v>
       </c>
       <c r="D8" t="str">
-        <v>B 304</v>
+        <v>A 1608</v>
       </c>
       <c r="E8" t="str">
         <v/>
       </c>
       <c r="F8" t="str">
-        <v>Til Poli x1</v>
+        <v>Wheat Chapati x1</v>
       </c>
       <c r="G8">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H8" t="str">
-        <v>COOKING</v>
+        <v>NEW</v>
       </c>
       <c r="I8" t="str">
         <v>PENDING</v>
       </c>
       <c r="J8" t="str">
+        <v>2026-01-13</v>
+      </c>
+      <c r="K8" t="str">
+        <v>15:50</v>
+      </c>
+      <c r="L8" t="str">
+        <v/>
+      </c>
+      <c r="M8" t="str">
+        <v/>
+      </c>
+      <c r="N8" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" t="str">
+        <v>2026-01-13 10:09</v>
+      </c>
+      <c r="C9" t="str">
+        <v>Anuradha N</v>
+      </c>
+      <c r="D9" t="str">
+        <v>B 304</v>
+      </c>
+      <c r="E9" t="str">
+        <v/>
+      </c>
+      <c r="F9" t="str">
+        <v>Til Poli x1</v>
+      </c>
+      <c r="G9">
+        <v>30</v>
+      </c>
+      <c r="H9" t="str">
+        <v>COOKING</v>
+      </c>
+      <c r="I9" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J9" t="str">
         <v>2026-01-14</v>
       </c>
-      <c r="K8" t="str">
+      <c r="K9" t="str">
         <v>16:45</v>
       </c>
-      <c r="L8" t="str">
-        <v/>
-      </c>
-      <c r="M8" t="str">
-        <v/>
-      </c>
-      <c r="N8" t="str">
+      <c r="L9" t="str">
+        <v/>
+      </c>
+      <c r="M9" t="str">
+        <v/>
+      </c>
+      <c r="N9" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N9"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -798,10 +842,10 @@
     </row>
     <row r="2">
       <c r="A2">
+        <v>8</v>
+      </c>
+      <c r="B2">
         <v>7</v>
-      </c>
-      <c r="B2">
-        <v>6</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -816,7 +860,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>195</v>
+        <v>215</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -831,7 +875,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -871,29 +915,40 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Onion Pakoda (Kanda Bhaje)</v>
+        <v>Jawar Bhakari</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4">
-        <v>60</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Pohe</v>
+        <v>Onion Pakoda (Kanda Bhaje)</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>Pohe</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
         <v>30</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
📊 Update SwaadSutra_Daily_2026-01-13.xlsx - 2026-01-13T19:05:20.387Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Daily_2026-01-13.xlsx
+++ b/reports/SwaadSutra_Daily_2026-01-13.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -450,25 +450,25 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" t="str">
-        <v>2026-01-13 18:59</v>
+        <v>2026-01-13 19:05</v>
       </c>
       <c r="C2" t="str">
         <v>Sagar Borse</v>
       </c>
       <c r="D2" t="str">
-        <v>A-1608</v>
+        <v>A1608</v>
       </c>
       <c r="E2" t="str">
         <v>7588930329</v>
       </c>
       <c r="F2" t="str">
-        <v>Jawar Bhakari x1</v>
+        <v>Wheat Chapati x1</v>
       </c>
       <c r="G2">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H2" t="str">
         <v>NEW</v>
@@ -477,10 +477,10 @@
         <v>PENDING</v>
       </c>
       <c r="J2" t="str">
-        <v>2026-01-16</v>
+        <v>2026-01-26</v>
       </c>
       <c r="K2" t="str">
-        <v>10:00</v>
+        <v>10:35</v>
       </c>
       <c r="L2" t="str">
         <v/>
@@ -494,25 +494,25 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" t="str">
-        <v>2026-01-13 16:54</v>
+        <v>2026-01-13 18:59</v>
       </c>
       <c r="C3" t="str">
-        <v>Pooja</v>
+        <v>Sagar Borse</v>
       </c>
       <c r="D3" t="str">
-        <v>a14</v>
+        <v>A-1608</v>
       </c>
       <c r="E3" t="str">
-        <v>9096648553</v>
+        <v>7588930329</v>
       </c>
       <c r="F3" t="str">
-        <v>Wheat Chapati x1</v>
+        <v>Jawar Bhakari x1</v>
       </c>
       <c r="G3">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H3" t="str">
         <v>NEW</v>
@@ -521,10 +521,10 @@
         <v>PENDING</v>
       </c>
       <c r="J3" t="str">
-        <v/>
+        <v>2026-01-16</v>
       </c>
       <c r="K3" t="str">
-        <v/>
+        <v>10:00</v>
       </c>
       <c r="L3" t="str">
         <v/>
@@ -538,16 +538,16 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" t="str">
-        <v>2026-01-13 16:41</v>
+        <v>2026-01-13 16:54</v>
       </c>
       <c r="C4" t="str">
         <v>Pooja</v>
       </c>
       <c r="D4" t="str">
-        <v>saf</v>
+        <v>a14</v>
       </c>
       <c r="E4" t="str">
         <v>9096648553</v>
@@ -565,10 +565,10 @@
         <v>PENDING</v>
       </c>
       <c r="J4" t="str">
-        <v>2026-01-15</v>
+        <v/>
       </c>
       <c r="K4" t="str">
-        <v>10:12</v>
+        <v/>
       </c>
       <c r="L4" t="str">
         <v/>
@@ -582,25 +582,25 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5" t="str">
-        <v>2026-01-13 16:40</v>
+        <v>2026-01-13 16:41</v>
       </c>
       <c r="C5" t="str">
-        <v>Sagar Borse</v>
+        <v>Pooja</v>
       </c>
       <c r="D5" t="str">
-        <v>A-1608</v>
+        <v>saf</v>
       </c>
       <c r="E5" t="str">
-        <v>7588930329</v>
+        <v>9096648553</v>
       </c>
       <c r="F5" t="str">
-        <v>Til Poli x1</v>
+        <v>Wheat Chapati x1</v>
       </c>
       <c r="G5">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H5" t="str">
         <v>NEW</v>
@@ -609,10 +609,10 @@
         <v>PENDING</v>
       </c>
       <c r="J5" t="str">
-        <v>2026-01-14</v>
+        <v>2026-01-15</v>
       </c>
       <c r="K5" t="str">
-        <v>10:00</v>
+        <v>10:12</v>
       </c>
       <c r="L5" t="str">
         <v/>
@@ -626,25 +626,25 @@
     </row>
     <row r="6">
       <c r="A6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" t="str">
-        <v>2026-01-13 16:39</v>
+        <v>2026-01-13 16:40</v>
       </c>
       <c r="C6" t="str">
-        <v>Pooja</v>
+        <v>Sagar Borse</v>
       </c>
       <c r="D6" t="str">
-        <v>A1608</v>
+        <v>A-1608</v>
       </c>
       <c r="E6" t="str">
-        <v>9096648553</v>
+        <v>7588930329</v>
       </c>
       <c r="F6" t="str">
-        <v>Onion Pakoda (Kanda Bhaje) x1</v>
+        <v>Til Poli x1</v>
       </c>
       <c r="G6">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="H6" t="str">
         <v>NEW</v>
@@ -656,7 +656,7 @@
         <v>2026-01-14</v>
       </c>
       <c r="K6" t="str">
-        <v>22:09</v>
+        <v>10:00</v>
       </c>
       <c r="L6" t="str">
         <v/>
@@ -670,25 +670,25 @@
     </row>
     <row r="7">
       <c r="A7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B7" t="str">
-        <v>2026-01-13 11:15</v>
+        <v>2026-01-13 16:39</v>
       </c>
       <c r="C7" t="str">
-        <v>Ajay Dwarkunde</v>
+        <v>Pooja</v>
       </c>
       <c r="D7" t="str">
-        <v>b-703</v>
+        <v>A1608</v>
       </c>
       <c r="E7" t="str">
-        <v>8087172173</v>
+        <v>9096648553</v>
       </c>
       <c r="F7" t="str">
-        <v>Pohe x1</v>
+        <v>Onion Pakoda (Kanda Bhaje) x1</v>
       </c>
       <c r="G7">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="H7" t="str">
         <v>NEW</v>
@@ -697,10 +697,10 @@
         <v>PENDING</v>
       </c>
       <c r="J7" t="str">
-        <v>2026-01-13</v>
+        <v>2026-01-14</v>
       </c>
       <c r="K7" t="str">
-        <v>18:50</v>
+        <v>22:09</v>
       </c>
       <c r="L7" t="str">
         <v/>
@@ -714,25 +714,25 @@
     </row>
     <row r="8">
       <c r="A8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B8" t="str">
-        <v>2026-01-13 10:20</v>
+        <v>2026-01-13 11:15</v>
       </c>
       <c r="C8" t="str">
-        <v>Pooja</v>
+        <v>Ajay Dwarkunde</v>
       </c>
       <c r="D8" t="str">
-        <v>A 1608</v>
+        <v>b-703</v>
       </c>
       <c r="E8" t="str">
-        <v/>
+        <v>8087172173</v>
       </c>
       <c r="F8" t="str">
-        <v>Wheat Chapati x1</v>
+        <v>Pohe x1</v>
       </c>
       <c r="G8">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="H8" t="str">
         <v>NEW</v>
@@ -744,7 +744,7 @@
         <v>2026-01-13</v>
       </c>
       <c r="K8" t="str">
-        <v>15:50</v>
+        <v>18:50</v>
       </c>
       <c r="L8" t="str">
         <v/>
@@ -758,51 +758,95 @@
     </row>
     <row r="9">
       <c r="A9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B9" t="str">
-        <v>2026-01-13 10:09</v>
+        <v>2026-01-13 10:20</v>
       </c>
       <c r="C9" t="str">
-        <v>Anuradha N</v>
+        <v>Pooja</v>
       </c>
       <c r="D9" t="str">
-        <v>B 304</v>
+        <v>A 1608</v>
       </c>
       <c r="E9" t="str">
         <v/>
       </c>
       <c r="F9" t="str">
-        <v>Til Poli x1</v>
+        <v>Wheat Chapati x1</v>
       </c>
       <c r="G9">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H9" t="str">
-        <v>COOKING</v>
+        <v>NEW</v>
       </c>
       <c r="I9" t="str">
         <v>PENDING</v>
       </c>
       <c r="J9" t="str">
+        <v>2026-01-13</v>
+      </c>
+      <c r="K9" t="str">
+        <v>15:50</v>
+      </c>
+      <c r="L9" t="str">
+        <v/>
+      </c>
+      <c r="M9" t="str">
+        <v/>
+      </c>
+      <c r="N9" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" t="str">
+        <v>2026-01-13 10:09</v>
+      </c>
+      <c r="C10" t="str">
+        <v>Anuradha N</v>
+      </c>
+      <c r="D10" t="str">
+        <v>B 304</v>
+      </c>
+      <c r="E10" t="str">
+        <v/>
+      </c>
+      <c r="F10" t="str">
+        <v>Til Poli x1</v>
+      </c>
+      <c r="G10">
+        <v>30</v>
+      </c>
+      <c r="H10" t="str">
+        <v>COOKING</v>
+      </c>
+      <c r="I10" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J10" t="str">
         <v>2026-01-14</v>
       </c>
-      <c r="K9" t="str">
+      <c r="K10" t="str">
         <v>16:45</v>
       </c>
-      <c r="L9" t="str">
-        <v/>
-      </c>
-      <c r="M9" t="str">
-        <v/>
-      </c>
-      <c r="N9" t="str">
+      <c r="L10" t="str">
+        <v/>
+      </c>
+      <c r="M10" t="str">
+        <v/>
+      </c>
+      <c r="N10" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N9"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N10"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -842,10 +886,10 @@
     </row>
     <row r="2">
       <c r="A2">
+        <v>9</v>
+      </c>
+      <c r="B2">
         <v>8</v>
-      </c>
-      <c r="B2">
-        <v>7</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -860,7 +904,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>215</v>
+        <v>230</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -896,10 +940,10 @@
         <v>Wheat Chapati</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2">
-        <v>45</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Daily_2026-01-13.xlsx - 2026-01-13T19:05:38.699Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Daily_2026-01-13.xlsx
+++ b/reports/SwaadSutra_Daily_2026-01-13.xlsx
@@ -471,7 +471,7 @@
         <v>15</v>
       </c>
       <c r="H2" t="str">
-        <v>NEW</v>
+        <v>COOKING</v>
       </c>
       <c r="I2" t="str">
         <v>PENDING</v>
@@ -889,10 +889,10 @@
         <v>9</v>
       </c>
       <c r="B2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2">
         <v>0</v>

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Daily_2026-01-13.xlsx - 2026-01-13T19:12:09.678Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Daily_2026-01-13.xlsx
+++ b/reports/SwaadSutra_Daily_2026-01-13.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -450,16 +450,16 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" t="str">
-        <v>2026-01-13 19:05</v>
+        <v>2026-01-13 19:12</v>
       </c>
       <c r="C2" t="str">
         <v>Sagar Borse</v>
       </c>
       <c r="D2" t="str">
-        <v>A1608</v>
+        <v>Yuu</v>
       </c>
       <c r="E2" t="str">
         <v>7588930329</v>
@@ -471,16 +471,16 @@
         <v>15</v>
       </c>
       <c r="H2" t="str">
-        <v>COOKING</v>
+        <v>NEW</v>
       </c>
       <c r="I2" t="str">
         <v>PENDING</v>
       </c>
       <c r="J2" t="str">
-        <v>2026-01-26</v>
+        <v>2026-01-15</v>
       </c>
       <c r="K2" t="str">
-        <v>10:35</v>
+        <v>02:42</v>
       </c>
       <c r="L2" t="str">
         <v/>
@@ -494,37 +494,37 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" t="str">
-        <v>2026-01-13 18:59</v>
+        <v>2026-01-13 19:05</v>
       </c>
       <c r="C3" t="str">
         <v>Sagar Borse</v>
       </c>
       <c r="D3" t="str">
-        <v>A-1608</v>
+        <v>A1608</v>
       </c>
       <c r="E3" t="str">
         <v>7588930329</v>
       </c>
       <c r="F3" t="str">
-        <v>Jawar Bhakari x1</v>
+        <v>Wheat Chapati x1</v>
       </c>
       <c r="G3">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H3" t="str">
-        <v>NEW</v>
+        <v>COOKING</v>
       </c>
       <c r="I3" t="str">
         <v>PENDING</v>
       </c>
       <c r="J3" t="str">
-        <v>2026-01-16</v>
+        <v>2026-01-26</v>
       </c>
       <c r="K3" t="str">
-        <v>10:00</v>
+        <v>10:35</v>
       </c>
       <c r="L3" t="str">
         <v/>
@@ -538,25 +538,25 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" t="str">
-        <v>2026-01-13 16:54</v>
+        <v>2026-01-13 18:59</v>
       </c>
       <c r="C4" t="str">
-        <v>Pooja</v>
+        <v>Sagar Borse</v>
       </c>
       <c r="D4" t="str">
-        <v>a14</v>
+        <v>A-1608</v>
       </c>
       <c r="E4" t="str">
-        <v>9096648553</v>
+        <v>7588930329</v>
       </c>
       <c r="F4" t="str">
-        <v>Wheat Chapati x1</v>
+        <v>Jawar Bhakari x1</v>
       </c>
       <c r="G4">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H4" t="str">
         <v>NEW</v>
@@ -565,10 +565,10 @@
         <v>PENDING</v>
       </c>
       <c r="J4" t="str">
-        <v/>
+        <v>2026-01-16</v>
       </c>
       <c r="K4" t="str">
-        <v/>
+        <v>10:00</v>
       </c>
       <c r="L4" t="str">
         <v/>
@@ -582,16 +582,16 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" t="str">
-        <v>2026-01-13 16:41</v>
+        <v>2026-01-13 16:54</v>
       </c>
       <c r="C5" t="str">
         <v>Pooja</v>
       </c>
       <c r="D5" t="str">
-        <v>saf</v>
+        <v>a14</v>
       </c>
       <c r="E5" t="str">
         <v>9096648553</v>
@@ -609,10 +609,10 @@
         <v>PENDING</v>
       </c>
       <c r="J5" t="str">
-        <v>2026-01-15</v>
+        <v/>
       </c>
       <c r="K5" t="str">
-        <v>10:12</v>
+        <v/>
       </c>
       <c r="L5" t="str">
         <v/>
@@ -626,25 +626,25 @@
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" t="str">
-        <v>2026-01-13 16:40</v>
+        <v>2026-01-13 16:41</v>
       </c>
       <c r="C6" t="str">
-        <v>Sagar Borse</v>
+        <v>Pooja</v>
       </c>
       <c r="D6" t="str">
-        <v>A-1608</v>
+        <v>saf</v>
       </c>
       <c r="E6" t="str">
-        <v>7588930329</v>
+        <v>9096648553</v>
       </c>
       <c r="F6" t="str">
-        <v>Til Poli x1</v>
+        <v>Wheat Chapati x1</v>
       </c>
       <c r="G6">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H6" t="str">
         <v>NEW</v>
@@ -653,10 +653,10 @@
         <v>PENDING</v>
       </c>
       <c r="J6" t="str">
-        <v>2026-01-14</v>
+        <v>2026-01-15</v>
       </c>
       <c r="K6" t="str">
-        <v>10:00</v>
+        <v>10:12</v>
       </c>
       <c r="L6" t="str">
         <v/>
@@ -670,25 +670,25 @@
     </row>
     <row r="7">
       <c r="A7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B7" t="str">
-        <v>2026-01-13 16:39</v>
+        <v>2026-01-13 16:40</v>
       </c>
       <c r="C7" t="str">
-        <v>Pooja</v>
+        <v>Sagar Borse</v>
       </c>
       <c r="D7" t="str">
-        <v>A1608</v>
+        <v>A-1608</v>
       </c>
       <c r="E7" t="str">
-        <v>9096648553</v>
+        <v>7588930329</v>
       </c>
       <c r="F7" t="str">
-        <v>Onion Pakoda (Kanda Bhaje) x1</v>
+        <v>Til Poli x1</v>
       </c>
       <c r="G7">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="H7" t="str">
         <v>NEW</v>
@@ -700,7 +700,7 @@
         <v>2026-01-14</v>
       </c>
       <c r="K7" t="str">
-        <v>22:09</v>
+        <v>10:00</v>
       </c>
       <c r="L7" t="str">
         <v/>
@@ -714,25 +714,25 @@
     </row>
     <row r="8">
       <c r="A8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B8" t="str">
-        <v>2026-01-13 11:15</v>
+        <v>2026-01-13 16:39</v>
       </c>
       <c r="C8" t="str">
-        <v>Ajay Dwarkunde</v>
+        <v>Pooja</v>
       </c>
       <c r="D8" t="str">
-        <v>b-703</v>
+        <v>A1608</v>
       </c>
       <c r="E8" t="str">
-        <v>8087172173</v>
+        <v>9096648553</v>
       </c>
       <c r="F8" t="str">
-        <v>Pohe x1</v>
+        <v>Onion Pakoda (Kanda Bhaje) x1</v>
       </c>
       <c r="G8">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="H8" t="str">
         <v>NEW</v>
@@ -741,10 +741,10 @@
         <v>PENDING</v>
       </c>
       <c r="J8" t="str">
-        <v>2026-01-13</v>
+        <v>2026-01-14</v>
       </c>
       <c r="K8" t="str">
-        <v>18:50</v>
+        <v>22:09</v>
       </c>
       <c r="L8" t="str">
         <v/>
@@ -758,25 +758,25 @@
     </row>
     <row r="9">
       <c r="A9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B9" t="str">
-        <v>2026-01-13 10:20</v>
+        <v>2026-01-13 11:15</v>
       </c>
       <c r="C9" t="str">
-        <v>Pooja</v>
+        <v>Ajay Dwarkunde</v>
       </c>
       <c r="D9" t="str">
-        <v>A 1608</v>
+        <v>b-703</v>
       </c>
       <c r="E9" t="str">
-        <v/>
+        <v>8087172173</v>
       </c>
       <c r="F9" t="str">
-        <v>Wheat Chapati x1</v>
+        <v>Pohe x1</v>
       </c>
       <c r="G9">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="H9" t="str">
         <v>NEW</v>
@@ -788,7 +788,7 @@
         <v>2026-01-13</v>
       </c>
       <c r="K9" t="str">
-        <v>15:50</v>
+        <v>18:50</v>
       </c>
       <c r="L9" t="str">
         <v/>
@@ -802,51 +802,95 @@
     </row>
     <row r="10">
       <c r="A10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B10" t="str">
-        <v>2026-01-13 10:09</v>
+        <v>2026-01-13 10:20</v>
       </c>
       <c r="C10" t="str">
-        <v>Anuradha N</v>
+        <v>Pooja</v>
       </c>
       <c r="D10" t="str">
-        <v>B 304</v>
+        <v>A 1608</v>
       </c>
       <c r="E10" t="str">
         <v/>
       </c>
       <c r="F10" t="str">
-        <v>Til Poli x1</v>
+        <v>Wheat Chapati x1</v>
       </c>
       <c r="G10">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H10" t="str">
-        <v>COOKING</v>
+        <v>NEW</v>
       </c>
       <c r="I10" t="str">
         <v>PENDING</v>
       </c>
       <c r="J10" t="str">
+        <v>2026-01-13</v>
+      </c>
+      <c r="K10" t="str">
+        <v>15:50</v>
+      </c>
+      <c r="L10" t="str">
+        <v/>
+      </c>
+      <c r="M10" t="str">
+        <v/>
+      </c>
+      <c r="N10" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="str">
+        <v>2026-01-13 10:09</v>
+      </c>
+      <c r="C11" t="str">
+        <v>Anuradha N</v>
+      </c>
+      <c r="D11" t="str">
+        <v>B 304</v>
+      </c>
+      <c r="E11" t="str">
+        <v/>
+      </c>
+      <c r="F11" t="str">
+        <v>Til Poli x1</v>
+      </c>
+      <c r="G11">
+        <v>30</v>
+      </c>
+      <c r="H11" t="str">
+        <v>COOKING</v>
+      </c>
+      <c r="I11" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J11" t="str">
         <v>2026-01-14</v>
       </c>
-      <c r="K10" t="str">
+      <c r="K11" t="str">
         <v>16:45</v>
       </c>
-      <c r="L10" t="str">
-        <v/>
-      </c>
-      <c r="M10" t="str">
-        <v/>
-      </c>
-      <c r="N10" t="str">
+      <c r="L11" t="str">
+        <v/>
+      </c>
+      <c r="M11" t="str">
+        <v/>
+      </c>
+      <c r="N11" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N10"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N11"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -886,10 +930,10 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2">
         <v>2</v>
@@ -904,7 +948,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>230</v>
+        <v>245</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -940,10 +984,10 @@
         <v>Wheat Chapati</v>
       </c>
       <c r="B2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2">
-        <v>60</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Daily_2026-01-13.xlsx - 2026-01-13T22:38:58.121Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Daily_2026-01-13.xlsx
+++ b/reports/SwaadSutra_Daily_2026-01-13.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -450,25 +450,25 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2" t="str">
-        <v>2026-01-13 19:12</v>
+        <v>2026-01-13 22:38</v>
       </c>
       <c r="C2" t="str">
-        <v>Sagar Borse</v>
+        <v>Phantom</v>
       </c>
       <c r="D2" t="str">
-        <v>Yuu</v>
+        <v>420</v>
       </c>
       <c r="E2" t="str">
-        <v>7588930329</v>
+        <v/>
       </c>
       <c r="F2" t="str">
-        <v>Wheat Chapati x1</v>
+        <v>Upma x1</v>
       </c>
       <c r="G2">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="H2" t="str">
         <v>NEW</v>
@@ -477,10 +477,10 @@
         <v>PENDING</v>
       </c>
       <c r="J2" t="str">
-        <v>2026-01-15</v>
+        <v>2026-01-14</v>
       </c>
       <c r="K2" t="str">
-        <v>02:42</v>
+        <v>15:38</v>
       </c>
       <c r="L2" t="str">
         <v/>
@@ -494,16 +494,16 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" t="str">
-        <v>2026-01-13 19:05</v>
+        <v>2026-01-13 19:12</v>
       </c>
       <c r="C3" t="str">
         <v>Sagar Borse</v>
       </c>
       <c r="D3" t="str">
-        <v>A1608</v>
+        <v>Yuu</v>
       </c>
       <c r="E3" t="str">
         <v>7588930329</v>
@@ -515,16 +515,16 @@
         <v>15</v>
       </c>
       <c r="H3" t="str">
-        <v>COOKING</v>
+        <v>NEW</v>
       </c>
       <c r="I3" t="str">
         <v>PENDING</v>
       </c>
       <c r="J3" t="str">
-        <v>2026-01-26</v>
+        <v>2026-01-15</v>
       </c>
       <c r="K3" t="str">
-        <v>10:35</v>
+        <v>02:42</v>
       </c>
       <c r="L3" t="str">
         <v/>
@@ -538,37 +538,37 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" t="str">
-        <v>2026-01-13 18:59</v>
+        <v>2026-01-13 19:05</v>
       </c>
       <c r="C4" t="str">
         <v>Sagar Borse</v>
       </c>
       <c r="D4" t="str">
-        <v>A-1608</v>
+        <v>A1608</v>
       </c>
       <c r="E4" t="str">
         <v>7588930329</v>
       </c>
       <c r="F4" t="str">
-        <v>Jawar Bhakari x1</v>
+        <v>Wheat Chapati x1</v>
       </c>
       <c r="G4">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H4" t="str">
-        <v>NEW</v>
+        <v>COOKING</v>
       </c>
       <c r="I4" t="str">
         <v>PENDING</v>
       </c>
       <c r="J4" t="str">
-        <v>2026-01-16</v>
+        <v>2026-01-26</v>
       </c>
       <c r="K4" t="str">
-        <v>10:00</v>
+        <v>10:35</v>
       </c>
       <c r="L4" t="str">
         <v/>
@@ -582,25 +582,25 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" t="str">
-        <v>2026-01-13 16:54</v>
+        <v>2026-01-13 18:59</v>
       </c>
       <c r="C5" t="str">
-        <v>Pooja</v>
+        <v>Sagar Borse</v>
       </c>
       <c r="D5" t="str">
-        <v>a14</v>
+        <v>A-1608</v>
       </c>
       <c r="E5" t="str">
-        <v>9096648553</v>
+        <v>7588930329</v>
       </c>
       <c r="F5" t="str">
-        <v>Wheat Chapati x1</v>
+        <v>Jawar Bhakari x1</v>
       </c>
       <c r="G5">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H5" t="str">
         <v>NEW</v>
@@ -609,10 +609,10 @@
         <v>PENDING</v>
       </c>
       <c r="J5" t="str">
-        <v/>
+        <v>2026-01-16</v>
       </c>
       <c r="K5" t="str">
-        <v/>
+        <v>10:00</v>
       </c>
       <c r="L5" t="str">
         <v/>
@@ -626,16 +626,16 @@
     </row>
     <row r="6">
       <c r="A6">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B6" t="str">
-        <v>2026-01-13 16:41</v>
+        <v>2026-01-13 16:54</v>
       </c>
       <c r="C6" t="str">
         <v>Pooja</v>
       </c>
       <c r="D6" t="str">
-        <v>saf</v>
+        <v>a14</v>
       </c>
       <c r="E6" t="str">
         <v>9096648553</v>
@@ -653,10 +653,10 @@
         <v>PENDING</v>
       </c>
       <c r="J6" t="str">
-        <v>2026-01-15</v>
+        <v/>
       </c>
       <c r="K6" t="str">
-        <v>10:12</v>
+        <v/>
       </c>
       <c r="L6" t="str">
         <v/>
@@ -670,25 +670,25 @@
     </row>
     <row r="7">
       <c r="A7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" t="str">
-        <v>2026-01-13 16:40</v>
+        <v>2026-01-13 16:41</v>
       </c>
       <c r="C7" t="str">
-        <v>Sagar Borse</v>
+        <v>Pooja</v>
       </c>
       <c r="D7" t="str">
-        <v>A-1608</v>
+        <v>saf</v>
       </c>
       <c r="E7" t="str">
-        <v>7588930329</v>
+        <v>9096648553</v>
       </c>
       <c r="F7" t="str">
-        <v>Til Poli x1</v>
+        <v>Wheat Chapati x1</v>
       </c>
       <c r="G7">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H7" t="str">
         <v>NEW</v>
@@ -697,10 +697,10 @@
         <v>PENDING</v>
       </c>
       <c r="J7" t="str">
-        <v>2026-01-14</v>
+        <v>2026-01-15</v>
       </c>
       <c r="K7" t="str">
-        <v>10:00</v>
+        <v>10:12</v>
       </c>
       <c r="L7" t="str">
         <v/>
@@ -714,25 +714,25 @@
     </row>
     <row r="8">
       <c r="A8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B8" t="str">
-        <v>2026-01-13 16:39</v>
+        <v>2026-01-13 16:40</v>
       </c>
       <c r="C8" t="str">
-        <v>Pooja</v>
+        <v>Sagar Borse</v>
       </c>
       <c r="D8" t="str">
-        <v>A1608</v>
+        <v>A-1608</v>
       </c>
       <c r="E8" t="str">
-        <v>9096648553</v>
+        <v>7588930329</v>
       </c>
       <c r="F8" t="str">
-        <v>Onion Pakoda (Kanda Bhaje) x1</v>
+        <v>Til Poli x1</v>
       </c>
       <c r="G8">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="H8" t="str">
         <v>NEW</v>
@@ -744,7 +744,7 @@
         <v>2026-01-14</v>
       </c>
       <c r="K8" t="str">
-        <v>22:09</v>
+        <v>10:00</v>
       </c>
       <c r="L8" t="str">
         <v/>
@@ -758,25 +758,25 @@
     </row>
     <row r="9">
       <c r="A9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B9" t="str">
-        <v>2026-01-13 11:15</v>
+        <v>2026-01-13 16:39</v>
       </c>
       <c r="C9" t="str">
-        <v>Ajay Dwarkunde</v>
+        <v>Pooja</v>
       </c>
       <c r="D9" t="str">
-        <v>b-703</v>
+        <v>A1608</v>
       </c>
       <c r="E9" t="str">
-        <v>8087172173</v>
+        <v>9096648553</v>
       </c>
       <c r="F9" t="str">
-        <v>Pohe x1</v>
+        <v>Onion Pakoda (Kanda Bhaje) x1</v>
       </c>
       <c r="G9">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="H9" t="str">
         <v>NEW</v>
@@ -785,10 +785,10 @@
         <v>PENDING</v>
       </c>
       <c r="J9" t="str">
-        <v>2026-01-13</v>
+        <v>2026-01-14</v>
       </c>
       <c r="K9" t="str">
-        <v>18:50</v>
+        <v>22:09</v>
       </c>
       <c r="L9" t="str">
         <v/>
@@ -802,25 +802,25 @@
     </row>
     <row r="10">
       <c r="A10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B10" t="str">
-        <v>2026-01-13 10:20</v>
+        <v>2026-01-13 11:15</v>
       </c>
       <c r="C10" t="str">
-        <v>Pooja</v>
+        <v>Ajay Dwarkunde</v>
       </c>
       <c r="D10" t="str">
-        <v>A 1608</v>
+        <v>b-703</v>
       </c>
       <c r="E10" t="str">
-        <v/>
+        <v>8087172173</v>
       </c>
       <c r="F10" t="str">
-        <v>Wheat Chapati x1</v>
+        <v>Pohe x1</v>
       </c>
       <c r="G10">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="H10" t="str">
         <v>NEW</v>
@@ -832,7 +832,7 @@
         <v>2026-01-13</v>
       </c>
       <c r="K10" t="str">
-        <v>15:50</v>
+        <v>18:50</v>
       </c>
       <c r="L10" t="str">
         <v/>
@@ -846,51 +846,95 @@
     </row>
     <row r="11">
       <c r="A11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B11" t="str">
-        <v>2026-01-13 10:09</v>
+        <v>2026-01-13 10:20</v>
       </c>
       <c r="C11" t="str">
-        <v>Anuradha N</v>
+        <v>Pooja</v>
       </c>
       <c r="D11" t="str">
-        <v>B 304</v>
+        <v>A 1608</v>
       </c>
       <c r="E11" t="str">
         <v/>
       </c>
       <c r="F11" t="str">
-        <v>Til Poli x1</v>
+        <v>Wheat Chapati x1</v>
       </c>
       <c r="G11">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H11" t="str">
-        <v>COOKING</v>
+        <v>NEW</v>
       </c>
       <c r="I11" t="str">
         <v>PENDING</v>
       </c>
       <c r="J11" t="str">
+        <v>2026-01-13</v>
+      </c>
+      <c r="K11" t="str">
+        <v>15:50</v>
+      </c>
+      <c r="L11" t="str">
+        <v/>
+      </c>
+      <c r="M11" t="str">
+        <v/>
+      </c>
+      <c r="N11" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12" t="str">
+        <v>2026-01-13 10:09</v>
+      </c>
+      <c r="C12" t="str">
+        <v>Anuradha N</v>
+      </c>
+      <c r="D12" t="str">
+        <v>B 304</v>
+      </c>
+      <c r="E12" t="str">
+        <v/>
+      </c>
+      <c r="F12" t="str">
+        <v>Til Poli x1</v>
+      </c>
+      <c r="G12">
+        <v>30</v>
+      </c>
+      <c r="H12" t="str">
+        <v>COOKING</v>
+      </c>
+      <c r="I12" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J12" t="str">
         <v>2026-01-14</v>
       </c>
-      <c r="K11" t="str">
+      <c r="K12" t="str">
         <v>16:45</v>
       </c>
-      <c r="L11" t="str">
-        <v/>
-      </c>
-      <c r="M11" t="str">
-        <v/>
-      </c>
-      <c r="N11" t="str">
+      <c r="L12" t="str">
+        <v/>
+      </c>
+      <c r="M12" t="str">
+        <v/>
+      </c>
+      <c r="N12" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N11"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N12"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -930,10 +974,10 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2">
         <v>2</v>
@@ -948,7 +992,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>245</v>
+        <v>275</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -963,7 +1007,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1003,40 +1047,51 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Jawar Bhakari</v>
+        <v>Upma</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Onion Pakoda (Kanda Bhaje)</v>
+        <v>Jawar Bhakari</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5">
-        <v>60</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>Pohe</v>
+        <v>Onion Pakoda (Kanda Bhaje)</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>Pohe</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
         <v>30</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C7"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
📊 Update SwaadSutra_Daily_2026-01-13.xlsx - 2026-01-13T22:43:06.768Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Daily_2026-01-13.xlsx
+++ b/reports/SwaadSutra_Daily_2026-01-13.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N12"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -450,13 +450,13 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" t="str">
-        <v>2026-01-13 22:38</v>
+        <v>2026-01-13 22:43</v>
       </c>
       <c r="C2" t="str">
-        <v>Phantom</v>
+        <v>Swapnil (Phantom)</v>
       </c>
       <c r="D2" t="str">
         <v>420</v>
@@ -465,10 +465,10 @@
         <v/>
       </c>
       <c r="F2" t="str">
-        <v>Upma x1</v>
+        <v>Vermicelli Kheer x1</v>
       </c>
       <c r="G2">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="H2" t="str">
         <v>NEW</v>
@@ -477,13 +477,13 @@
         <v>PENDING</v>
       </c>
       <c r="J2" t="str">
-        <v>2026-01-14</v>
+        <v>2026-01-15</v>
       </c>
       <c r="K2" t="str">
-        <v>15:38</v>
+        <v>16:42</v>
       </c>
       <c r="L2" t="str">
-        <v/>
+        <v>No vermicelli in kheer please.</v>
       </c>
       <c r="M2" t="str">
         <v/>
@@ -494,25 +494,25 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" t="str">
-        <v>2026-01-13 19:12</v>
+        <v>2026-01-13 22:38</v>
       </c>
       <c r="C3" t="str">
-        <v>Sagar Borse</v>
+        <v>Phantom</v>
       </c>
       <c r="D3" t="str">
-        <v>Yuu</v>
+        <v>420</v>
       </c>
       <c r="E3" t="str">
-        <v>7588930329</v>
+        <v/>
       </c>
       <c r="F3" t="str">
-        <v>Wheat Chapati x1</v>
+        <v>Upma x1</v>
       </c>
       <c r="G3">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="H3" t="str">
         <v>NEW</v>
@@ -521,10 +521,10 @@
         <v>PENDING</v>
       </c>
       <c r="J3" t="str">
-        <v>2026-01-15</v>
+        <v>2026-01-14</v>
       </c>
       <c r="K3" t="str">
-        <v>02:42</v>
+        <v>15:38</v>
       </c>
       <c r="L3" t="str">
         <v/>
@@ -538,16 +538,16 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" t="str">
-        <v>2026-01-13 19:05</v>
+        <v>2026-01-13 19:12</v>
       </c>
       <c r="C4" t="str">
         <v>Sagar Borse</v>
       </c>
       <c r="D4" t="str">
-        <v>A1608</v>
+        <v>Yuu</v>
       </c>
       <c r="E4" t="str">
         <v>7588930329</v>
@@ -559,16 +559,16 @@
         <v>15</v>
       </c>
       <c r="H4" t="str">
-        <v>COOKING</v>
+        <v>NEW</v>
       </c>
       <c r="I4" t="str">
         <v>PENDING</v>
       </c>
       <c r="J4" t="str">
-        <v>2026-01-26</v>
+        <v>2026-01-15</v>
       </c>
       <c r="K4" t="str">
-        <v>10:35</v>
+        <v>02:42</v>
       </c>
       <c r="L4" t="str">
         <v/>
@@ -582,37 +582,37 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" t="str">
-        <v>2026-01-13 18:59</v>
+        <v>2026-01-13 19:05</v>
       </c>
       <c r="C5" t="str">
         <v>Sagar Borse</v>
       </c>
       <c r="D5" t="str">
-        <v>A-1608</v>
+        <v>A1608</v>
       </c>
       <c r="E5" t="str">
         <v>7588930329</v>
       </c>
       <c r="F5" t="str">
-        <v>Jawar Bhakari x1</v>
+        <v>Wheat Chapati x1</v>
       </c>
       <c r="G5">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H5" t="str">
-        <v>NEW</v>
+        <v>COOKING</v>
       </c>
       <c r="I5" t="str">
         <v>PENDING</v>
       </c>
       <c r="J5" t="str">
-        <v>2026-01-16</v>
+        <v>2026-01-26</v>
       </c>
       <c r="K5" t="str">
-        <v>10:00</v>
+        <v>10:35</v>
       </c>
       <c r="L5" t="str">
         <v/>
@@ -626,25 +626,25 @@
     </row>
     <row r="6">
       <c r="A6">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B6" t="str">
-        <v>2026-01-13 16:54</v>
+        <v>2026-01-13 18:59</v>
       </c>
       <c r="C6" t="str">
-        <v>Pooja</v>
+        <v>Sagar Borse</v>
       </c>
       <c r="D6" t="str">
-        <v>a14</v>
+        <v>A-1608</v>
       </c>
       <c r="E6" t="str">
-        <v>9096648553</v>
+        <v>7588930329</v>
       </c>
       <c r="F6" t="str">
-        <v>Wheat Chapati x1</v>
+        <v>Jawar Bhakari x1</v>
       </c>
       <c r="G6">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H6" t="str">
         <v>NEW</v>
@@ -653,10 +653,10 @@
         <v>PENDING</v>
       </c>
       <c r="J6" t="str">
-        <v/>
+        <v>2026-01-16</v>
       </c>
       <c r="K6" t="str">
-        <v/>
+        <v>10:00</v>
       </c>
       <c r="L6" t="str">
         <v/>
@@ -670,16 +670,16 @@
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7" t="str">
-        <v>2026-01-13 16:41</v>
+        <v>2026-01-13 16:54</v>
       </c>
       <c r="C7" t="str">
         <v>Pooja</v>
       </c>
       <c r="D7" t="str">
-        <v>saf</v>
+        <v>a14</v>
       </c>
       <c r="E7" t="str">
         <v>9096648553</v>
@@ -697,10 +697,10 @@
         <v>PENDING</v>
       </c>
       <c r="J7" t="str">
-        <v>2026-01-15</v>
+        <v/>
       </c>
       <c r="K7" t="str">
-        <v>10:12</v>
+        <v/>
       </c>
       <c r="L7" t="str">
         <v/>
@@ -714,25 +714,25 @@
     </row>
     <row r="8">
       <c r="A8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B8" t="str">
-        <v>2026-01-13 16:40</v>
+        <v>2026-01-13 16:41</v>
       </c>
       <c r="C8" t="str">
-        <v>Sagar Borse</v>
+        <v>Pooja</v>
       </c>
       <c r="D8" t="str">
-        <v>A-1608</v>
+        <v>saf</v>
       </c>
       <c r="E8" t="str">
-        <v>7588930329</v>
+        <v>9096648553</v>
       </c>
       <c r="F8" t="str">
-        <v>Til Poli x1</v>
+        <v>Wheat Chapati x1</v>
       </c>
       <c r="G8">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H8" t="str">
         <v>NEW</v>
@@ -741,10 +741,10 @@
         <v>PENDING</v>
       </c>
       <c r="J8" t="str">
-        <v>2026-01-14</v>
+        <v>2026-01-15</v>
       </c>
       <c r="K8" t="str">
-        <v>10:00</v>
+        <v>10:12</v>
       </c>
       <c r="L8" t="str">
         <v/>
@@ -758,25 +758,25 @@
     </row>
     <row r="9">
       <c r="A9">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B9" t="str">
-        <v>2026-01-13 16:39</v>
+        <v>2026-01-13 16:40</v>
       </c>
       <c r="C9" t="str">
-        <v>Pooja</v>
+        <v>Sagar Borse</v>
       </c>
       <c r="D9" t="str">
-        <v>A1608</v>
+        <v>A-1608</v>
       </c>
       <c r="E9" t="str">
-        <v>9096648553</v>
+        <v>7588930329</v>
       </c>
       <c r="F9" t="str">
-        <v>Onion Pakoda (Kanda Bhaje) x1</v>
+        <v>Til Poli x1</v>
       </c>
       <c r="G9">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="H9" t="str">
         <v>NEW</v>
@@ -788,7 +788,7 @@
         <v>2026-01-14</v>
       </c>
       <c r="K9" t="str">
-        <v>22:09</v>
+        <v>10:00</v>
       </c>
       <c r="L9" t="str">
         <v/>
@@ -802,25 +802,25 @@
     </row>
     <row r="10">
       <c r="A10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B10" t="str">
-        <v>2026-01-13 11:15</v>
+        <v>2026-01-13 16:39</v>
       </c>
       <c r="C10" t="str">
-        <v>Ajay Dwarkunde</v>
+        <v>Pooja</v>
       </c>
       <c r="D10" t="str">
-        <v>b-703</v>
+        <v>A1608</v>
       </c>
       <c r="E10" t="str">
-        <v>8087172173</v>
+        <v>9096648553</v>
       </c>
       <c r="F10" t="str">
-        <v>Pohe x1</v>
+        <v>Onion Pakoda (Kanda Bhaje) x1</v>
       </c>
       <c r="G10">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="H10" t="str">
         <v>NEW</v>
@@ -829,10 +829,10 @@
         <v>PENDING</v>
       </c>
       <c r="J10" t="str">
-        <v>2026-01-13</v>
+        <v>2026-01-14</v>
       </c>
       <c r="K10" t="str">
-        <v>18:50</v>
+        <v>22:09</v>
       </c>
       <c r="L10" t="str">
         <v/>
@@ -846,25 +846,25 @@
     </row>
     <row r="11">
       <c r="A11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B11" t="str">
-        <v>2026-01-13 10:20</v>
+        <v>2026-01-13 11:15</v>
       </c>
       <c r="C11" t="str">
-        <v>Pooja</v>
+        <v>Ajay Dwarkunde</v>
       </c>
       <c r="D11" t="str">
-        <v>A 1608</v>
+        <v>b-703</v>
       </c>
       <c r="E11" t="str">
-        <v/>
+        <v>8087172173</v>
       </c>
       <c r="F11" t="str">
-        <v>Wheat Chapati x1</v>
+        <v>Pohe x1</v>
       </c>
       <c r="G11">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="H11" t="str">
         <v>NEW</v>
@@ -876,7 +876,7 @@
         <v>2026-01-13</v>
       </c>
       <c r="K11" t="str">
-        <v>15:50</v>
+        <v>18:50</v>
       </c>
       <c r="L11" t="str">
         <v/>
@@ -890,51 +890,95 @@
     </row>
     <row r="12">
       <c r="A12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B12" t="str">
-        <v>2026-01-13 10:09</v>
+        <v>2026-01-13 10:20</v>
       </c>
       <c r="C12" t="str">
-        <v>Anuradha N</v>
+        <v>Pooja</v>
       </c>
       <c r="D12" t="str">
-        <v>B 304</v>
+        <v>A 1608</v>
       </c>
       <c r="E12" t="str">
         <v/>
       </c>
       <c r="F12" t="str">
-        <v>Til Poli x1</v>
+        <v>Wheat Chapati x1</v>
       </c>
       <c r="G12">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H12" t="str">
-        <v>COOKING</v>
+        <v>NEW</v>
       </c>
       <c r="I12" t="str">
         <v>PENDING</v>
       </c>
       <c r="J12" t="str">
+        <v>2026-01-13</v>
+      </c>
+      <c r="K12" t="str">
+        <v>15:50</v>
+      </c>
+      <c r="L12" t="str">
+        <v/>
+      </c>
+      <c r="M12" t="str">
+        <v/>
+      </c>
+      <c r="N12" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13" t="str">
+        <v>2026-01-13 10:09</v>
+      </c>
+      <c r="C13" t="str">
+        <v>Anuradha N</v>
+      </c>
+      <c r="D13" t="str">
+        <v>B 304</v>
+      </c>
+      <c r="E13" t="str">
+        <v/>
+      </c>
+      <c r="F13" t="str">
+        <v>Til Poli x1</v>
+      </c>
+      <c r="G13">
+        <v>30</v>
+      </c>
+      <c r="H13" t="str">
+        <v>COOKING</v>
+      </c>
+      <c r="I13" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J13" t="str">
         <v>2026-01-14</v>
       </c>
-      <c r="K12" t="str">
+      <c r="K13" t="str">
         <v>16:45</v>
       </c>
-      <c r="L12" t="str">
-        <v/>
-      </c>
-      <c r="M12" t="str">
-        <v/>
-      </c>
-      <c r="N12" t="str">
+      <c r="L13" t="str">
+        <v/>
+      </c>
+      <c r="M13" t="str">
+        <v/>
+      </c>
+      <c r="N13" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N12"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N13"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -974,10 +1018,10 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2">
         <v>2</v>
@@ -992,7 +1036,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>275</v>
+        <v>325</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -1007,7 +1051,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1047,51 +1091,62 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Upma</v>
+        <v>Vermicelli Kheer</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4">
-        <v>30</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Jawar Bhakari</v>
+        <v>Upma</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>Onion Pakoda (Kanda Bhaje)</v>
+        <v>Jawar Bhakari</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6">
-        <v>60</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>Pohe</v>
+        <v>Onion Pakoda (Kanda Bhaje)</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>Pohe</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
         <v>30</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C8"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
📊 Update SwaadSutra_Daily_2026-01-13.xlsx - 2026-01-13T22:51:28.908Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Daily_2026-01-13.xlsx
+++ b/reports/SwaadSutra_Daily_2026-01-13.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -450,25 +450,25 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" t="str">
-        <v>2026-01-13 22:43</v>
+        <v>2026-01-13 22:51</v>
       </c>
       <c r="C2" t="str">
-        <v>Swapnil (Phantom)</v>
+        <v>Ketki</v>
       </c>
       <c r="D2" t="str">
-        <v>420</v>
+        <v>1608</v>
       </c>
       <c r="E2" t="str">
-        <v/>
+        <v>3159135521</v>
       </c>
       <c r="F2" t="str">
-        <v>Vermicelli Kheer x1</v>
+        <v>Wheat Chapati x1</v>
       </c>
       <c r="G2">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="H2" t="str">
         <v>NEW</v>
@@ -477,13 +477,13 @@
         <v>PENDING</v>
       </c>
       <c r="J2" t="str">
-        <v>2026-01-15</v>
+        <v>2026-01-14</v>
       </c>
       <c r="K2" t="str">
-        <v>16:42</v>
+        <v>16:51</v>
       </c>
       <c r="L2" t="str">
-        <v>No vermicelli in kheer please.</v>
+        <v/>
       </c>
       <c r="M2" t="str">
         <v/>
@@ -494,13 +494,13 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3" t="str">
-        <v>2026-01-13 22:38</v>
+        <v>2026-01-13 22:43</v>
       </c>
       <c r="C3" t="str">
-        <v>Phantom</v>
+        <v>Swapnil (Phantom)</v>
       </c>
       <c r="D3" t="str">
         <v>420</v>
@@ -509,10 +509,10 @@
         <v/>
       </c>
       <c r="F3" t="str">
-        <v>Upma x1</v>
+        <v>Vermicelli Kheer x1</v>
       </c>
       <c r="G3">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="H3" t="str">
         <v>NEW</v>
@@ -521,13 +521,13 @@
         <v>PENDING</v>
       </c>
       <c r="J3" t="str">
-        <v>2026-01-14</v>
+        <v>2026-01-15</v>
       </c>
       <c r="K3" t="str">
-        <v>15:38</v>
+        <v>16:42</v>
       </c>
       <c r="L3" t="str">
-        <v/>
+        <v>No vermicelli in kheer please.</v>
       </c>
       <c r="M3" t="str">
         <v/>
@@ -538,25 +538,25 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" t="str">
-        <v>2026-01-13 19:12</v>
+        <v>2026-01-13 22:38</v>
       </c>
       <c r="C4" t="str">
-        <v>Sagar Borse</v>
+        <v>Phantom</v>
       </c>
       <c r="D4" t="str">
-        <v>Yuu</v>
+        <v>420</v>
       </c>
       <c r="E4" t="str">
-        <v>7588930329</v>
+        <v/>
       </c>
       <c r="F4" t="str">
-        <v>Wheat Chapati x1</v>
+        <v>Upma x1</v>
       </c>
       <c r="G4">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="H4" t="str">
         <v>NEW</v>
@@ -565,10 +565,10 @@
         <v>PENDING</v>
       </c>
       <c r="J4" t="str">
-        <v>2026-01-15</v>
+        <v>2026-01-14</v>
       </c>
       <c r="K4" t="str">
-        <v>02:42</v>
+        <v>15:38</v>
       </c>
       <c r="L4" t="str">
         <v/>
@@ -582,16 +582,16 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5" t="str">
-        <v>2026-01-13 19:05</v>
+        <v>2026-01-13 19:12</v>
       </c>
       <c r="C5" t="str">
         <v>Sagar Borse</v>
       </c>
       <c r="D5" t="str">
-        <v>A1608</v>
+        <v>Yuu</v>
       </c>
       <c r="E5" t="str">
         <v>7588930329</v>
@@ -603,16 +603,16 @@
         <v>15</v>
       </c>
       <c r="H5" t="str">
-        <v>COOKING</v>
+        <v>NEW</v>
       </c>
       <c r="I5" t="str">
         <v>PENDING</v>
       </c>
       <c r="J5" t="str">
-        <v>2026-01-26</v>
+        <v>2026-01-15</v>
       </c>
       <c r="K5" t="str">
-        <v>10:35</v>
+        <v>02:42</v>
       </c>
       <c r="L5" t="str">
         <v/>
@@ -626,37 +626,37 @@
     </row>
     <row r="6">
       <c r="A6">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" t="str">
-        <v>2026-01-13 18:59</v>
+        <v>2026-01-13 19:05</v>
       </c>
       <c r="C6" t="str">
         <v>Sagar Borse</v>
       </c>
       <c r="D6" t="str">
-        <v>A-1608</v>
+        <v>A1608</v>
       </c>
       <c r="E6" t="str">
         <v>7588930329</v>
       </c>
       <c r="F6" t="str">
-        <v>Jawar Bhakari x1</v>
+        <v>Wheat Chapati x1</v>
       </c>
       <c r="G6">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H6" t="str">
-        <v>NEW</v>
+        <v>COOKING</v>
       </c>
       <c r="I6" t="str">
         <v>PENDING</v>
       </c>
       <c r="J6" t="str">
-        <v>2026-01-16</v>
+        <v>2026-01-26</v>
       </c>
       <c r="K6" t="str">
-        <v>10:00</v>
+        <v>10:35</v>
       </c>
       <c r="L6" t="str">
         <v/>
@@ -670,25 +670,25 @@
     </row>
     <row r="7">
       <c r="A7">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B7" t="str">
-        <v>2026-01-13 16:54</v>
+        <v>2026-01-13 18:59</v>
       </c>
       <c r="C7" t="str">
-        <v>Pooja</v>
+        <v>Sagar Borse</v>
       </c>
       <c r="D7" t="str">
-        <v>a14</v>
+        <v>A-1608</v>
       </c>
       <c r="E7" t="str">
-        <v>9096648553</v>
+        <v>7588930329</v>
       </c>
       <c r="F7" t="str">
-        <v>Wheat Chapati x1</v>
+        <v>Jawar Bhakari x1</v>
       </c>
       <c r="G7">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H7" t="str">
         <v>NEW</v>
@@ -697,10 +697,10 @@
         <v>PENDING</v>
       </c>
       <c r="J7" t="str">
-        <v/>
+        <v>2026-01-16</v>
       </c>
       <c r="K7" t="str">
-        <v/>
+        <v>10:00</v>
       </c>
       <c r="L7" t="str">
         <v/>
@@ -714,16 +714,16 @@
     </row>
     <row r="8">
       <c r="A8">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" t="str">
-        <v>2026-01-13 16:41</v>
+        <v>2026-01-13 16:54</v>
       </c>
       <c r="C8" t="str">
         <v>Pooja</v>
       </c>
       <c r="D8" t="str">
-        <v>saf</v>
+        <v>a14</v>
       </c>
       <c r="E8" t="str">
         <v>9096648553</v>
@@ -741,10 +741,10 @@
         <v>PENDING</v>
       </c>
       <c r="J8" t="str">
-        <v>2026-01-15</v>
+        <v/>
       </c>
       <c r="K8" t="str">
-        <v>10:12</v>
+        <v/>
       </c>
       <c r="L8" t="str">
         <v/>
@@ -758,25 +758,25 @@
     </row>
     <row r="9">
       <c r="A9">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B9" t="str">
-        <v>2026-01-13 16:40</v>
+        <v>2026-01-13 16:41</v>
       </c>
       <c r="C9" t="str">
-        <v>Sagar Borse</v>
+        <v>Pooja</v>
       </c>
       <c r="D9" t="str">
-        <v>A-1608</v>
+        <v>saf</v>
       </c>
       <c r="E9" t="str">
-        <v>7588930329</v>
+        <v>9096648553</v>
       </c>
       <c r="F9" t="str">
-        <v>Til Poli x1</v>
+        <v>Wheat Chapati x1</v>
       </c>
       <c r="G9">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H9" t="str">
         <v>NEW</v>
@@ -785,10 +785,10 @@
         <v>PENDING</v>
       </c>
       <c r="J9" t="str">
-        <v>2026-01-14</v>
+        <v>2026-01-15</v>
       </c>
       <c r="K9" t="str">
-        <v>10:00</v>
+        <v>10:12</v>
       </c>
       <c r="L9" t="str">
         <v/>
@@ -802,25 +802,25 @@
     </row>
     <row r="10">
       <c r="A10">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B10" t="str">
-        <v>2026-01-13 16:39</v>
+        <v>2026-01-13 16:40</v>
       </c>
       <c r="C10" t="str">
-        <v>Pooja</v>
+        <v>Sagar Borse</v>
       </c>
       <c r="D10" t="str">
-        <v>A1608</v>
+        <v>A-1608</v>
       </c>
       <c r="E10" t="str">
-        <v>9096648553</v>
+        <v>7588930329</v>
       </c>
       <c r="F10" t="str">
-        <v>Onion Pakoda (Kanda Bhaje) x1</v>
+        <v>Til Poli x1</v>
       </c>
       <c r="G10">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="H10" t="str">
         <v>NEW</v>
@@ -832,7 +832,7 @@
         <v>2026-01-14</v>
       </c>
       <c r="K10" t="str">
-        <v>22:09</v>
+        <v>10:00</v>
       </c>
       <c r="L10" t="str">
         <v/>
@@ -846,25 +846,25 @@
     </row>
     <row r="11">
       <c r="A11">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B11" t="str">
-        <v>2026-01-13 11:15</v>
+        <v>2026-01-13 16:39</v>
       </c>
       <c r="C11" t="str">
-        <v>Ajay Dwarkunde</v>
+        <v>Pooja</v>
       </c>
       <c r="D11" t="str">
-        <v>b-703</v>
+        <v>A1608</v>
       </c>
       <c r="E11" t="str">
-        <v>8087172173</v>
+        <v>9096648553</v>
       </c>
       <c r="F11" t="str">
-        <v>Pohe x1</v>
+        <v>Onion Pakoda (Kanda Bhaje) x1</v>
       </c>
       <c r="G11">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="H11" t="str">
         <v>NEW</v>
@@ -873,10 +873,10 @@
         <v>PENDING</v>
       </c>
       <c r="J11" t="str">
-        <v>2026-01-13</v>
+        <v>2026-01-14</v>
       </c>
       <c r="K11" t="str">
-        <v>18:50</v>
+        <v>22:09</v>
       </c>
       <c r="L11" t="str">
         <v/>
@@ -890,25 +890,25 @@
     </row>
     <row r="12">
       <c r="A12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B12" t="str">
-        <v>2026-01-13 10:20</v>
+        <v>2026-01-13 11:15</v>
       </c>
       <c r="C12" t="str">
-        <v>Pooja</v>
+        <v>Ajay Dwarkunde</v>
       </c>
       <c r="D12" t="str">
-        <v>A 1608</v>
+        <v>b-703</v>
       </c>
       <c r="E12" t="str">
-        <v/>
+        <v>8087172173</v>
       </c>
       <c r="F12" t="str">
-        <v>Wheat Chapati x1</v>
+        <v>Pohe x1</v>
       </c>
       <c r="G12">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="H12" t="str">
         <v>NEW</v>
@@ -920,7 +920,7 @@
         <v>2026-01-13</v>
       </c>
       <c r="K12" t="str">
-        <v>15:50</v>
+        <v>18:50</v>
       </c>
       <c r="L12" t="str">
         <v/>
@@ -934,51 +934,95 @@
     </row>
     <row r="13">
       <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13" t="str">
+        <v>2026-01-13 10:20</v>
+      </c>
+      <c r="C13" t="str">
+        <v>Pooja</v>
+      </c>
+      <c r="D13" t="str">
+        <v>A 1608</v>
+      </c>
+      <c r="E13" t="str">
+        <v/>
+      </c>
+      <c r="F13" t="str">
+        <v>Wheat Chapati x1</v>
+      </c>
+      <c r="G13">
+        <v>15</v>
+      </c>
+      <c r="H13" t="str">
+        <v>NEW</v>
+      </c>
+      <c r="I13" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J13" t="str">
+        <v>2026-01-13</v>
+      </c>
+      <c r="K13" t="str">
+        <v>15:50</v>
+      </c>
+      <c r="L13" t="str">
+        <v/>
+      </c>
+      <c r="M13" t="str">
+        <v/>
+      </c>
+      <c r="N13" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14">
         <v>1</v>
       </c>
-      <c r="B13" t="str">
+      <c r="B14" t="str">
         <v>2026-01-13 10:09</v>
       </c>
-      <c r="C13" t="str">
+      <c r="C14" t="str">
         <v>Anuradha N</v>
       </c>
-      <c r="D13" t="str">
+      <c r="D14" t="str">
         <v>B 304</v>
       </c>
-      <c r="E13" t="str">
-        <v/>
-      </c>
-      <c r="F13" t="str">
+      <c r="E14" t="str">
+        <v/>
+      </c>
+      <c r="F14" t="str">
         <v>Til Poli x1</v>
       </c>
-      <c r="G13">
+      <c r="G14">
         <v>30</v>
       </c>
-      <c r="H13" t="str">
+      <c r="H14" t="str">
         <v>COOKING</v>
       </c>
-      <c r="I13" t="str">
-        <v>PENDING</v>
-      </c>
-      <c r="J13" t="str">
+      <c r="I14" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J14" t="str">
         <v>2026-01-14</v>
       </c>
-      <c r="K13" t="str">
+      <c r="K14" t="str">
         <v>16:45</v>
       </c>
-      <c r="L13" t="str">
-        <v/>
-      </c>
-      <c r="M13" t="str">
-        <v/>
-      </c>
-      <c r="N13" t="str">
+      <c r="L14" t="str">
+        <v/>
+      </c>
+      <c r="M14" t="str">
+        <v/>
+      </c>
+      <c r="N14" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N13"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N14"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -1018,10 +1062,10 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2">
         <v>2</v>
@@ -1036,7 +1080,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>325</v>
+        <v>340</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -1072,10 +1116,10 @@
         <v>Wheat Chapati</v>
       </c>
       <c r="B2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3">

</xml_diff>